<commit_message>
Alterada planilha e removidos imports desnecessários
</commit_message>
<xml_diff>
--- a/public/Eletronica - 2 semestre.xlsx
+++ b/public/Eletronica - 2 semestre.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailan Patrick\Desktop\Gerador de Boletins Incluir\boletim_email\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailan Patrick\Desktop\Gerador de Boletins Incluir\boletim-por-email-incluir\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5314956E-F34F-4635-A999-4BED3CF96A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D92C93-4B80-496B-A4CD-AAF952FC5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="36">
   <si>
     <t>PROFESSORES: Frederico Marazzi Xavier Firmo, Monitores: Julio Cesar, Gabriel Groppo</t>
   </si>
@@ -145,12 +145,15 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <t>Eletônica - 1 Semestre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +194,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF9900"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -379,9 +389,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection sqref="A1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -639,133 +649,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="20"/>
+      <c r="A1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="22"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="26" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="27" t="s">
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="26" t="s">
+      <c r="U3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="V3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="28" t="s">
+      <c r="W3" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="27" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="26" t="s">
+      <c r="S4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="23"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="22"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -805,15 +817,15 @@
       <c r="N5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="23"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
corrigido bug após a alteração da planilha
</commit_message>
<xml_diff>
--- a/public/Eletronica - 2 semestre.xlsx
+++ b/public/Eletronica - 2 semestre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailan Patrick\Desktop\Gerador de Boletins Incluir\boletim-por-email-incluir\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D92C93-4B80-496B-A4CD-AAF952FC5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2E15B-1CA5-4E14-9968-6B5A9EF0033E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,14 +146,14 @@
     <t>F</t>
   </si>
   <si>
-    <t>Eletônica - 1 Semestre</t>
+    <t>Eletrônica - 1 Semestre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,6 +201,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF9900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -338,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,6 +396,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,7 +419,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -649,135 +659,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="25" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="26" t="s">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="V3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="26" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="25" t="s">
+      <c r="R4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="25" t="s">
+      <c r="S4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -817,15 +827,15 @@
       <c r="N5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="23"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1382,14 +1392,24 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="O13" s="29">
+        <v>25</v>
+      </c>
+      <c r="P13" s="29">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>8</v>
+      </c>
+      <c r="R13" s="29">
+        <v>10</v>
+      </c>
+      <c r="S13" s="29">
+        <v>200</v>
+      </c>
       <c r="T13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="U13" s="5">
         <f t="shared" si="4"/>
@@ -1397,7 +1417,7 @@
       </c>
       <c r="V13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>REPROVADO</v>
+        <v>APROVADO</v>
       </c>
       <c r="W13" s="6"/>
     </row>

</xml_diff>